<commit_message>
Diagrama de clases a mitad
</commit_message>
<xml_diff>
--- a/4.-Documentación/Entidades.xlsx
+++ b/4.-Documentación/Entidades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\mega\2.-CursosyApuntes\DesarrollodeAplicacionesMultiplataforma\1.-Proyectofinalmodulo\4.-Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA5BEC4-ACFB-4473-9A2F-6810DC6F0120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19B34F1-ACAF-4F78-8645-55E2130B3927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8625" yWindow="675" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="2025" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
   <si>
     <t>empleado</t>
   </si>
@@ -81,9 +81,6 @@
     <t>servicio</t>
   </si>
   <si>
-    <t>id_Servicio</t>
-  </si>
-  <si>
     <t>fecha</t>
   </si>
   <si>
@@ -108,9 +105,6 @@
     <t>Deficiencia</t>
   </si>
   <si>
-    <t>id_Deficiencia</t>
-  </si>
-  <si>
     <t>solucion</t>
   </si>
   <si>
@@ -129,18 +123,12 @@
     <t>Alerta</t>
   </si>
   <si>
-    <t>id_Alerta</t>
-  </si>
-  <si>
     <t>resuelta</t>
   </si>
   <si>
     <t>Item</t>
   </si>
   <si>
-    <t>id_Item</t>
-  </si>
-  <si>
     <t>fabricante</t>
   </si>
   <si>
@@ -153,9 +141,6 @@
     <t>Color</t>
   </si>
   <si>
-    <t>id_Marca</t>
-  </si>
-  <si>
     <t>id_Modelo</t>
   </si>
   <si>
@@ -169,6 +154,9 @@
   </si>
   <si>
     <t>id_Cliente</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -212,10 +200,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,7 +486,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A6" sqref="A6:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,13 +546,13 @@
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G2" t="s">
         <v>15</v>
@@ -574,7 +561,7 @@
         <v>16</v>
       </c>
       <c r="I2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -582,90 +569,84 @@
         <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
       </c>
       <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
       <c r="F3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="D5" t="s">
         <v>27</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>28</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>29</v>
       </c>
-      <c r="E5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" t="s">
-        <v>31</v>
-      </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F7" t="s">
         <v>12</v>
@@ -673,16 +654,16 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
@@ -690,10 +671,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
@@ -701,7 +682,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>43</v>
@@ -712,10 +693,10 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
@@ -723,10 +704,10 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C12" t="s">
         <v>3</v>

</xml_diff>